<commit_message>
Finalizou nas alterações no Modelo
</commit_message>
<xml_diff>
--- a/infosis.xlsx
+++ b/infosis.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="43">
   <si>
     <t>nome</t>
   </si>
@@ -139,6 +139,27 @@
   </si>
   <si>
     <t>2019-01-01 13:00:00.000</t>
+  </si>
+  <si>
+    <t>José</t>
+  </si>
+  <si>
+    <t>Carlos</t>
+  </si>
+  <si>
+    <t>145.609.357-69</t>
+  </si>
+  <si>
+    <t>PJ</t>
+  </si>
+  <si>
+    <t>Desenvolvedor Mobile</t>
+  </si>
+  <si>
+    <t>Ana</t>
+  </si>
+  <si>
+    <t>500.000.145-33</t>
   </si>
 </sst>
 </file>
@@ -274,7 +295,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -322,6 +343,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -636,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -999,6 +1023,52 @@
         <v>17</v>
       </c>
     </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="16"/>
+      <c r="E14" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" s="6">
+        <v>8</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="16"/>
+      <c r="E15" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" s="6">
+        <v>8</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>